<commit_message>
Cambio en archivo de ejemplp
</commit_message>
<xml_diff>
--- a/examples/data1.xlsx
+++ b/examples/data1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="912" windowWidth="18036" windowHeight="7068"/>
+    <workbookView xWindow="0" yWindow="1368" windowWidth="18036" windowHeight="7068"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -77,7 +77,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
-    <numFmt numFmtId="166" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -116,7 +116,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -436,7 +436,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C12"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>